<commit_message>
Work related to Diarmuid Early post
</commit_message>
<xml_diff>
--- a/LambdaForProgressiveTaxCalculations.xlsx
+++ b/LambdaForProgressiveTaxCalculations.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{FF17B754-0A69-4751-A7FB-B752B946ACB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{386A3F75-8B03-46F6-81F9-D28265F5E1E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-57705" yWindow="-2730" windowWidth="29010" windowHeight="18015" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
+    <workbookView xWindow="-54720" yWindow="-1185" windowWidth="25725" windowHeight="16260" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="4" r:id="rId1"/>
+    <sheet name="InitialLook" sheetId="4" r:id="rId1"/>
     <sheet name="Formats" sheetId="2" r:id="rId2"/>
     <sheet name="Lists" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -23,7 +23,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="7" r:id="rId4"/>
+    <pivotCache cacheId="8" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,6 +36,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -65,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="28">
   <si>
     <t>FROM:</t>
   </si>
@@ -146,6 +148,9 @@
   </si>
   <si>
     <t>New lambda function for gist</t>
+  </si>
+  <si>
+    <t>Alternative Calculation</t>
   </si>
 </sst>
 </file>
@@ -340,9 +345,9 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="3"/>
   </cellXfs>
   <cellStyles count="14">
     <cellStyle name="Comment" xfId="9" xr:uid="{C4DDEBC2-DCD2-4316-AAE7-A5F6C47DBA99}"/>
@@ -637,6 +642,175 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>56</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="2" name="Group 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A251028D-9F84-4440-94BD-ED590FEF1134}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="3063240" cy="514406"/>
+          <a:chOff x="3162301" y="274265"/>
+          <a:chExt cx="3067050" cy="502976"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="3" name="TextBox 2">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C17F3E0F-3729-C82B-B828-1FB33F1BEF5B}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3162301" y="274265"/>
+            <a:ext cx="809778" cy="502976"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="accent3">
+              <a:lumMod val="40000"/>
+              <a:lumOff val="60000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln w="9525" cmpd="sng">
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="91440" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="1"/>
+              <a:t>FROM:</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="1"/>
+              <a:t>SUBJECT:</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="1"/>
+              <a:t>DATE:</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="4" name="TextBox 3">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{32B6302B-0237-47BD-9327-67786A435512}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3908004" y="274265"/>
+            <a:ext cx="2321347" cy="502976"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="bg2"/>
+          </a:solidFill>
+          <a:ln w="9525" cmpd="sng">
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="91440" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="0"/>
+              <a:t>Mark Biegert</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="0"/>
+              <a:t>Progressive Tax Calculator</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="0"/>
+              <a:t>12-Jun-2024</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -764,7 +938,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F44C8824-5739-49B7-BCFF-9C42983375DF}" name="PivotTable1" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F44C8824-5739-49B7-BCFF-9C42983375DF}" name="PivotTable1" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
   <location ref="B17:F28" firstHeaderRow="1" firstDataRow="2" firstDataCol="2"/>
   <pivotFields count="4">
     <pivotField axis="axisRow" compact="0" showAll="0" defaultSubtotal="0">
@@ -1069,6 +1243,9 @@
   <we:bindings/>
   <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
   <we:extLst>
+    <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{D87F86FE-615C-45B5-9D79-34F1136793EB}">
+      <we:containsCustomFunctions/>
+    </a:ext>
     <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{7C84B067-C214-45C3-A712-C9D94CD141B2}">
       <we:customFunctionIdList>
         <we:customFunctionIds>_xldudf_LABS_GENERATIVEAI</we:customFunctionIds>
@@ -1080,10 +1257,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E19A21DE-AE5C-4466-B858-0D1F67BCF639}">
-  <dimension ref="B1:I14"/>
+  <dimension ref="A5:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1093,104 +1270,141 @@
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
+    <row r="5" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
         <v>24</v>
       </c>
-      <c r="C1">
+      <c r="C7">
         <v>140000</v>
       </c>
-    </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
+      <c r="H7" s="11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
         <v>21</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C9" t="s">
         <v>22</v>
       </c>
-      <c r="I3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B4">
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B10">
         <v>0</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C10" s="9">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="11">
+      <c r="H10" s="10">
         <v>20550</v>
       </c>
-      <c r="C5" s="10">
+      <c r="I10">
+        <f>H10*C10</f>
+        <v>2055</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B11" s="10">
+        <v>20550</v>
+      </c>
+      <c r="C11" s="9">
         <v>0.12</v>
       </c>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="11">
+      <c r="H11" s="10">
+        <f>B12-B11</f>
+        <v>63000</v>
+      </c>
+      <c r="I11">
+        <f>C11*H11</f>
+        <v>7560</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B12" s="10">
         <v>83550</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C12" s="9">
         <v>0.22</v>
       </c>
-    </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B7" s="11">
+      <c r="H12" s="10">
+        <f>MIN(B13-B12,C7-B12)</f>
+        <v>56450</v>
+      </c>
+      <c r="I12">
+        <f>H12*C12</f>
+        <v>12419</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B13" s="10">
         <v>178150</v>
       </c>
-      <c r="C7" s="10">
+      <c r="C13" s="9">
         <v>0.24</v>
       </c>
-    </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B8" s="11">
+      <c r="H13" s="10">
+        <f>SUM(H10:H12)</f>
+        <v>140000</v>
+      </c>
+      <c r="I13">
+        <f>SUM(I10:I12)</f>
+        <v>22034</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B14" s="10">
         <v>340100</v>
       </c>
-      <c r="C8" s="10">
+      <c r="C14" s="9">
         <v>0.32</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B9" s="11">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B15" s="10">
         <v>431900</v>
       </c>
-      <c r="C9" s="10">
+      <c r="C15" s="9">
         <v>0.35</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="11">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B16" s="10">
         <v>647850</v>
       </c>
-      <c r="C10" s="10">
+      <c r="C16" s="9">
         <v>0.37</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
         <v>26</v>
       </c>
-      <c r="E12" cm="1">
-        <f t="array" ref="E12">taxCalc(C1,B4:B10,C4:C10)</f>
+      <c r="E18" cm="1">
+        <f t="array" ref="E18">taxCalc(C7,B10:B16,C10:C16)</f>
         <v>22034</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
         <v>25</v>
       </c>
-      <c r="E14" cm="1">
-        <f t="array" ref="E14">_xlfn.LAMBDA(_xlpm.income,_xlpm.brackLow,_xlpm.rat,
+      <c r="E20" cm="1">
+        <f t="array" ref="E20">_xlfn.LAMBDA(_xlpm.income,_xlpm.brackLow,_xlpm.rat,
     _xlfn.LET(_xlpm.brackHigh,_xlfn.VSTACK(_xlfn.DROP(_xlpm.brackLow,1),_xlpm.income),
         _xlpm.inBand,IF(_xlpm.income&lt;_xlpm.brackLow,0,IF(_xlpm.income&gt;_xlpm.brackHigh,_xlpm.brackHigh,_xlpm.income)-_xlpm.brackLow),
-        SUM(_xlpm.inBand*_xlpm.rat)))(C1,B4:B10,C4:C10)</f>
+        SUM(_xlpm.inBand*_xlpm.rat)))(C7,B10:B16,C10:C16)</f>
         <v>22034</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1202,7 +1416,7 @@
   <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1368,19 +1582,15 @@
       <c r="B19" t="s">
         <v>8</v>
       </c>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C20">
         <v>1</v>
       </c>
-      <c r="D20" s="9">
+      <c r="D20">
         <v>1</v>
       </c>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9">
+      <c r="F20">
         <v>1</v>
       </c>
     </row>
@@ -1388,11 +1598,10 @@
       <c r="C21">
         <v>2</v>
       </c>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9">
+      <c r="E21">
         <v>2</v>
       </c>
-      <c r="F21" s="9">
+      <c r="F21">
         <v>2</v>
       </c>
     </row>
@@ -1400,19 +1609,15 @@
       <c r="B22" t="s">
         <v>9</v>
       </c>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C23">
         <v>1</v>
       </c>
-      <c r="D23" s="9">
+      <c r="D23">
         <v>3</v>
       </c>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9">
+      <c r="F23">
         <v>3</v>
       </c>
     </row>
@@ -1420,11 +1625,10 @@
       <c r="C24">
         <v>2</v>
       </c>
-      <c r="D24" s="9"/>
-      <c r="E24" s="9">
+      <c r="E24">
         <v>4</v>
       </c>
-      <c r="F24" s="9">
+      <c r="F24">
         <v>4</v>
       </c>
     </row>
@@ -1432,19 +1636,15 @@
       <c r="B25" t="s">
         <v>10</v>
       </c>
-      <c r="D25" s="9"/>
-      <c r="E25" s="9"/>
-      <c r="F25" s="9"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C26">
         <v>1</v>
       </c>
-      <c r="D26" s="9">
+      <c r="D26">
         <v>5</v>
       </c>
-      <c r="E26" s="9"/>
-      <c r="F26" s="9">
+      <c r="F26">
         <v>5</v>
       </c>
     </row>
@@ -1452,11 +1652,10 @@
       <c r="C27">
         <v>2</v>
       </c>
-      <c r="D27" s="9"/>
-      <c r="E27" s="9">
+      <c r="E27">
         <v>6</v>
       </c>
-      <c r="F27" s="9">
+      <c r="F27">
         <v>6</v>
       </c>
     </row>
@@ -1464,13 +1663,13 @@
       <c r="B28" t="s">
         <v>13</v>
       </c>
-      <c r="D28" s="9">
+      <c r="D28">
         <v>9</v>
       </c>
-      <c r="E28" s="9">
+      <c r="E28">
         <v>12</v>
       </c>
-      <c r="F28" s="9">
+      <c r="F28">
         <v>21</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Compute effective tax rate
</commit_message>
<xml_diff>
--- a/LambdaForProgressiveTaxCalculations.xlsx
+++ b/LambdaForProgressiveTaxCalculations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F67A9261-79BA-4156-8EFF-A7BED7AADCE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AAF3EA6-3AC0-4F08-8299-7D33506A6E18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-30720" yWindow="-450" windowWidth="28830" windowHeight="17775" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
   </bookViews>
@@ -23,7 +23,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="16" r:id="rId4"/>
+    <pivotCache cacheId="17" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="32">
   <si>
     <t>FROM:</t>
   </si>
@@ -160,12 +160,18 @@
   </si>
   <si>
     <t>Calculation Work</t>
+  </si>
+  <si>
+    <t>Effective Tax Rate</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0%"/>
+  </numFmts>
   <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -345,7 +351,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="14">
+  <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
@@ -360,8 +366,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="7"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="8"/>
@@ -377,8 +384,9 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="12"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="14" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="14">
+  <cellStyles count="15">
     <cellStyle name="Comment" xfId="9" xr:uid="{C4DDEBC2-DCD2-4316-AAE7-A5F6C47DBA99}"/>
     <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" customBuiltin="1"/>
@@ -391,6 +399,7 @@
     <cellStyle name="Intro_Value" xfId="8" xr:uid="{15DF3F31-B3CA-47B9-81DE-6CDBDA24C6D7}"/>
     <cellStyle name="Linked Cell" xfId="10" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
+    <cellStyle name="Percent" xfId="14" builtinId="5"/>
     <cellStyle name="Title" xfId="1" builtinId="15" hidden="1"/>
     <cellStyle name="Total" xfId="6" builtinId="25" customBuiltin="1"/>
   </cellStyles>
@@ -840,13 +849,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>440992</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>51</xdr:row>
       <xdr:rowOff>98511</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1011,7 +1020,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F44C8824-5739-49B7-BCFF-9C42983375DF}" name="PivotTable1" cacheId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F44C8824-5739-49B7-BCFF-9C42983375DF}" name="PivotTable1" cacheId="17" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
   <location ref="B17:F28" firstHeaderRow="1" firstDataRow="2" firstDataCol="2"/>
   <pivotFields count="4">
     <pivotField axis="axisRow" compact="0" showAll="0" defaultSubtotal="0">
@@ -1330,10 +1339,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E19A21DE-AE5C-4466-B858-0D1F67BCF639}">
-  <dimension ref="A5:I24"/>
+  <dimension ref="A5:I25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N15" sqref="N15"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1468,29 +1477,38 @@
         <v>22034</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
         <v>25</v>
       </c>
-      <c r="E21" cm="1">
-        <f t="array" ref="E21">_xlfn.LAMBDA(_xlpm.income,_xlpm.brackLow,_xlpm.rat,
+      <c r="E20" cm="1">
+        <f t="array" ref="E20">_xlfn.LAMBDA(_xlpm.income,_xlpm.brackLow,_xlpm.rat,
     _xlfn.LET(_xlpm.brackHigh,_xlfn.VSTACK(_xlfn.DROP(_xlpm.brackLow,1),_xlpm.income),
         _xlpm.inBand,IF(_xlpm.income&lt;_xlpm.brackLow,0,IF(_xlpm.income&gt;_xlpm.brackHigh,_xlpm.brackHigh,_xlpm.income)-_xlpm.brackLow),
         SUM(_xlpm.inBand*_xlpm.rat)))(C9,B11:B17,C11:C17)</f>
         <v>22034</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A24" s="4" t="s">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>31</v>
+      </c>
+      <c r="E21" s="15">
+        <f>E19/C9</f>
+        <v>0.1573857142857143</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A25" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C24" s="12" t="s">
+      <c r="C25" s="12" t="s">
         <v>29</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C24" r:id="rId1" xr:uid="{BFFE080A-AD5C-4D9E-897C-5AB9E1CAE9EA}"/>
+    <hyperlink ref="C25" r:id="rId1" xr:uid="{BFFE080A-AD5C-4D9E-897C-5AB9E1CAE9EA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId2"/>

</xml_diff>